<commit_message>
implement oop for google pkg
</commit_message>
<xml_diff>
--- a/certificates.xlsx
+++ b/certificates.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="614">
   <si>
     <t>Date</t>
   </si>
@@ -1623,9 +1623,6 @@
     <t>d329fb86a98533895cc9</t>
   </si>
   <si>
-    <t>drive.google.com/file/d/1PAzBkAcEVOe-Y-YtqqaWFsAPoHVdrZju/view</t>
-  </si>
-  <si>
     <t>d329fb86a98533895cc967dcae966e81c1704bd665227e866aa2243d40f860d1</t>
   </si>
   <si>
@@ -1833,211 +1830,31 @@
     <t>drive.google.com/file/d/1VjeyDVI6HeuvIazF3ZRSJTAK1Oj9jlmL/view</t>
   </si>
   <si>
-    <t>5cd7fc5bd09930ef70c4</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/1lervrTjn3jFFJB8OoBg3tYjUe-LavtZu/view</t>
-  </si>
-  <si>
-    <t>93620030db08953cbf17468ffde46134834b7da10958b5174e935d4e324ce081</t>
-  </si>
-  <si>
-    <t>5cd7fc5bd09930ef70c4e7e58a6a83f278c99e7d5951d421fb1652154546e5ff</t>
-  </si>
-  <si>
-    <t>G029ROzmBqnsBCQZmBLyFqwpglcoomCleh7cH6bHLecGMkidlGujjtz8Zy9m/eyHdFTNmsoDN01Vvtfr9KjWWpE=</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/1Fpp3woPJahAxbsEmbGc3y3RwwNgWM9Z_/view</t>
-  </si>
-  <si>
-    <t>a527181b18ed3314770d</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/1BUf8V82jFUtTSeaPI7umBhi5fs_azyIS/view</t>
-  </si>
-  <si>
-    <t>b3240a1974bff838f35320554f851b14ea2bd31f46bcb893a35546b7ea8b3112</t>
-  </si>
-  <si>
-    <t>a527181b18ed3314770d19153878f7e5aa584f14a87e4ff7359e0f786d111035</t>
-  </si>
-  <si>
-    <t>HEOkbyz8bDIFPyt2qLyQKiF6PtZS8wREgFyhz4O54wtqCgzQKt5A4/mqu/ChtsP/wKGSUjVaJdHYmbDV6J6lr0g=</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/1WLCZ0IgrsPTDh1jszQy-AL8bIwPI8fn2/view</t>
-  </si>
-  <si>
     <t>14.12.2022</t>
   </si>
   <si>
-    <t>3b04927f55902a2ce8d1</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/1z41m5MP3Z3NnOh2994FlKddz5IGA2fGh/view</t>
-  </si>
-  <si>
-    <t>b94492feb30efb7f94082666a936891a31a43de0e18af1aa8a110ef869532d93</t>
-  </si>
-  <si>
-    <t>3b04927f55902a2ce8d1f9931139403d76b7347dbd9b7b6a6f1175ed0f80f941</t>
-  </si>
-  <si>
-    <t>G1Af8g1usQE9Wk+50wmPFuq9q6NpEu8OraZB1XidUTeiWNTGikuvuMOWFqJbVQCyQbz82XJ1HdhVWNfChHCM4Ts=</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/1PJ7OiX4ESeHFmnBOlTOV9mypK2ffduhp/view</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pasha Charovatiy</t>
   </si>
   <si>
-    <t>6afd8584d5a31bd08cb5</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/13VFwbzYvHdoVPIJpVFS5zVhfay1iYguY/view</t>
-  </si>
-  <si>
-    <t>151f4183ce68ec59b82ccbef71ac6f538e0eb86354c29ded27bca54fa4b95c99</t>
-  </si>
-  <si>
-    <t>6afd8584d5a31bd08cb5299a9eadf98b32dd8fd340ef5e7cc2a3d0338cdb9553</t>
-  </si>
-  <si>
-    <t>GwbTQ558Ef1Qmbjpamvebq+xa4iD9kUagVoWfYeSh7hAQbImq3LiZzMT5h6LQW1xBcQFBu8/ArIV2Sh799tnojc=</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/1F8hyY2ZM61utkPbNVJuXi4yrWnVAEGwQ/view</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dmytro Serhiienko</t>
   </si>
   <si>
-    <t>239235b8877849babd00</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/1wuMcWCw21CjGclyddT5wGzZmZnTCxZO0/view</t>
-  </si>
-  <si>
-    <t>42bdd76bce3b85dabf4bdba92100db768bf64e72f2b3535930b69bef40aa3c4c</t>
-  </si>
-  <si>
-    <t>239235b8877849babd005c0bdc00e5141e181216ca9761d6042537838537a92a</t>
-  </si>
-  <si>
-    <t>G3y2skz1RxbOpoRGpzorMBMiQ0l7TZ5HPLxYmOAiZ1hmBrDgyXuSMX2K1E/82HiAXrVn+XZn1qqSvsC7zvhzxok=</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/1qRMBdxumqIX6mxQoRlofWfUGz4P3Jbp3/view</t>
-  </si>
-  <si>
     <t xml:space="preserve">Vladislav Dmitrenko</t>
   </si>
   <si>
-    <t>6216890da62268a69ccb</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/12mhD3MWVhmzenFixvjs9euvoT0HlszHL/view</t>
-  </si>
-  <si>
-    <t>890c4726435f6d5a1c10068273e8dd8a3ac0645a9564bbf149f0d74a891669c6</t>
-  </si>
-  <si>
-    <t>6216890da62268a69ccbe039022f0738af441806a2f1b3093cf0f1d8454ccb30</t>
-  </si>
-  <si>
-    <t>G38acOrQBdbLXCuUxSFO9lALbfsfBpO/EAIugej0SbbiWocA/HhUfhDm2sfzk5CPDetE70H8b5ml4p89fl+5NLg=</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/1t7SFjfdNdVazwML8SM2gkmvFsbvIGf57/view</t>
-  </si>
-  <si>
     <t xml:space="preserve">Marina Rindina</t>
   </si>
   <si>
-    <t>17e586906755f2233b1c</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/1zI1rFcSy3DPnqyKUF7Nk48aJonfL6NEd/view</t>
-  </si>
-  <si>
-    <t>05f89d361327d9ef1679342cb8ed0488715da550cba8f0bdc7160caa43b5929c</t>
-  </si>
-  <si>
-    <t>17e586906755f2233b1cec389b9cdb1af335724ae1a3a3541aeda7908fbec6ab</t>
-  </si>
-  <si>
-    <t>HFeYSABLqPUIGNVrL/gUrQyuoN8mYz86RsbrfI3iked4M/KsMFznj/LGmBdJlYbsyD0ZbMegMt+U6tH3Aop1NG0=</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/1U0JKz1B2RADbxKll6VKzdSMFZ6ip_UuD/view</t>
-  </si>
-  <si>
     <t>15.12.2022</t>
   </si>
   <si>
     <t xml:space="preserve">Nazar Franko</t>
   </si>
   <si>
-    <t>5fce9047bf62cc2c4f27</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/1k6pv-RdvNR7oD8ZeXS5aQ-sRiThxFkEv/view</t>
-  </si>
-  <si>
-    <t>fec88d795aed9c59a04f91dedb06380fd764c753a54d6bdb96cea82b6ba05e29</t>
-  </si>
-  <si>
-    <t>5fce9047bf62cc2c4f27564f5a90b61aee2365834b9b6b7f6ba6832d6b29f036</t>
-  </si>
-  <si>
-    <t>HCErOToWnoQlZxTLcboCM35Seo7tDbUUdpdDxeENBmWJIO8+957D1z6rNg+CXpXVqb0w6U/zwlBtDNvMq2OO27A=</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/1dJHqOtnWFvKqrHoL4Tqq7rcBjp1G_WaA/view</t>
-  </si>
-  <si>
     <t xml:space="preserve">Olha Drahomeretska</t>
   </si>
   <si>
-    <t>0b67879057bfd2f3c6e1</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/1OyBBPvFLU5O_ssa9NrEI_Eb5GvonCwQI/view</t>
-  </si>
-  <si>
-    <t>9b293cc55ae62c9db4d9ce36cbc12b07e861f9c2cc1fdea2619f10ceca7aa779</t>
-  </si>
-  <si>
-    <t>0b67879057bfd2f3c6e1e9d3fa743bdc4d78a53501c96c4e5f184e105db7b17c</t>
-  </si>
-  <si>
-    <t>HDrYvaIx2k5Fier1DitF4GT3hKIeLkczjWyuvk+/cKuJZb3ICfssn/9NxN3Th5orxelFkAkgT3wORkxRIwCPBkk=</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/1Lk3e4Yex2W1dwzwisWhwKuLrXPElV_Eq/view</t>
-  </si>
-  <si>
     <t xml:space="preserve">Maksym Cherniak</t>
-  </si>
-  <si>
-    <t>e85ddb3ff95fb1668446</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/1FQCoo9V_ZkuOu-Yr4lCDsWiz1WHbmBfj/view</t>
-  </si>
-  <si>
-    <t>ac2b88ac92caf80b12076489c877b91785360487aa3135871883e597da139682</t>
-  </si>
-  <si>
-    <t>e85ddb3ff95fb166844688499268e6c6d4efffb6c2eb571cbb21e2ffafe57162</t>
-  </si>
-  <si>
-    <t>G3gfVxP3ewHz6dP2Z+0N1/qt4aK6N/0en1Qx25F3mwS7c3qT5LwPhJ+XE+kby5liifLyVH8z3nAZ3jKQc/9YgP0=</t>
-  </si>
-  <si>
-    <t>drive.google.com/file/d/1558dIA8mr9-mbKfPAiPR9CKmNYFMozdH/view</t>
   </si>
 </sst>
 </file>
@@ -2696,7 +2513,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A1" zoomScale="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
@@ -7154,20 +6971,18 @@
       <c r="E103" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="F103" s="16" t="s">
+      <c r="F103" s="16"/>
+      <c r="G103" s="6" t="s">
         <v>536</v>
-      </c>
-      <c r="G103" s="6" t="s">
-        <v>537</v>
       </c>
       <c r="H103" s="5" t="s">
         <v>150</v>
       </c>
       <c r="I103" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="J103" s="17" t="s">
         <v>538</v>
-      </c>
-      <c r="J103" s="17" t="s">
-        <v>539</v>
       </c>
       <c r="K103" s="4"/>
       <c r="L103" s="4"/>
@@ -7194,26 +7009,26 @@
         <v>431</v>
       </c>
       <c r="C104" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="D104" s="11" t="s">
         <v>540</v>
-      </c>
-      <c r="D104" s="11" t="s">
-        <v>541</v>
       </c>
       <c r="E104" s="4"/>
       <c r="F104" s="16" t="s">
+        <v>541</v>
+      </c>
+      <c r="G104" s="6" t="s">
         <v>542</v>
       </c>
-      <c r="G104" s="6" t="s">
+      <c r="H104" s="5" t="s">
         <v>543</v>
       </c>
-      <c r="H104" s="5" t="s">
+      <c r="I104" s="6" t="s">
         <v>544</v>
       </c>
-      <c r="I104" s="6" t="s">
+      <c r="J104" s="17" t="s">
         <v>545</v>
-      </c>
-      <c r="J104" s="17" t="s">
-        <v>546</v>
       </c>
       <c r="K104" s="4"/>
       <c r="L104" s="4"/>
@@ -7234,7 +7049,7 @@
     </row>
     <row r="105">
       <c r="A105" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>431</v>
@@ -7243,25 +7058,25 @@
         <v>505</v>
       </c>
       <c r="D105" s="11" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E105" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F105" s="16" t="s">
+        <v>548</v>
+      </c>
+      <c r="G105" s="6" t="s">
         <v>549</v>
       </c>
-      <c r="G105" s="6" t="s">
+      <c r="H105" s="5" t="s">
         <v>550</v>
       </c>
-      <c r="H105" s="5" t="s">
+      <c r="I105" s="6" t="s">
         <v>551</v>
       </c>
-      <c r="I105" s="6" t="s">
+      <c r="J105" s="17" t="s">
         <v>552</v>
-      </c>
-      <c r="J105" s="17" t="s">
-        <v>553</v>
       </c>
       <c r="K105" s="4"/>
       <c r="L105" s="4"/>
@@ -7282,34 +7097,34 @@
     </row>
     <row r="106">
       <c r="A106" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>505</v>
       </c>
       <c r="D106" s="11" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F106" s="16" t="s">
+        <v>555</v>
+      </c>
+      <c r="G106" s="6" t="s">
         <v>556</v>
-      </c>
-      <c r="G106" s="6" t="s">
-        <v>557</v>
       </c>
       <c r="H106" s="5" t="s">
         <v>150</v>
       </c>
       <c r="I106" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="J106" s="17" t="s">
         <v>558</v>
-      </c>
-      <c r="J106" s="17" t="s">
-        <v>559</v>
       </c>
       <c r="K106" s="4"/>
       <c r="L106" s="4"/>
@@ -7330,7 +7145,7 @@
     </row>
     <row r="107">
       <c r="A107" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>374</v>
@@ -7339,23 +7154,23 @@
         <v>505</v>
       </c>
       <c r="D107" s="11" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E107" s="4"/>
       <c r="F107" s="16" t="s">
+        <v>561</v>
+      </c>
+      <c r="G107" s="6" t="s">
         <v>562</v>
       </c>
-      <c r="G107" s="6" t="s">
+      <c r="H107" s="5" t="s">
         <v>563</v>
       </c>
-      <c r="H107" s="5" t="s">
+      <c r="I107" s="6" t="s">
         <v>564</v>
       </c>
-      <c r="I107" s="6" t="s">
+      <c r="J107" s="17" t="s">
         <v>565</v>
-      </c>
-      <c r="J107" s="17" t="s">
-        <v>566</v>
       </c>
       <c r="K107" s="4"/>
       <c r="L107" s="4"/>
@@ -7376,32 +7191,32 @@
     </row>
     <row r="108">
       <c r="A108" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>505</v>
       </c>
       <c r="D108" s="11" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E108" s="4"/>
       <c r="F108" s="16" t="s">
+        <v>568</v>
+      </c>
+      <c r="G108" s="6" t="s">
         <v>569</v>
       </c>
-      <c r="G108" s="6" t="s">
+      <c r="H108" s="5" t="s">
         <v>570</v>
       </c>
-      <c r="H108" s="5" t="s">
+      <c r="I108" s="6" t="s">
         <v>571</v>
       </c>
-      <c r="I108" s="6" t="s">
+      <c r="J108" s="17" t="s">
         <v>572</v>
-      </c>
-      <c r="J108" s="17" t="s">
-        <v>573</v>
       </c>
       <c r="K108" s="4"/>
       <c r="L108" s="4"/>
@@ -7422,34 +7237,34 @@
     </row>
     <row r="109">
       <c r="A109" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>505</v>
       </c>
       <c r="D109" s="11" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E109" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F109" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="G109" s="6" t="s">
         <v>576</v>
-      </c>
-      <c r="G109" s="6" t="s">
-        <v>577</v>
       </c>
       <c r="H109" s="5" t="s">
         <v>150</v>
       </c>
       <c r="I109" s="6" t="s">
+        <v>577</v>
+      </c>
+      <c r="J109" s="17" t="s">
         <v>578</v>
-      </c>
-      <c r="J109" s="17" t="s">
-        <v>579</v>
       </c>
       <c r="K109" s="4"/>
       <c r="L109" s="4"/>
@@ -7470,34 +7285,34 @@
     </row>
     <row r="110">
       <c r="A110" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>505</v>
       </c>
       <c r="D110" s="11" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E110" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F110" s="16" t="s">
+        <v>581</v>
+      </c>
+      <c r="G110" s="6" t="s">
         <v>582</v>
-      </c>
-      <c r="G110" s="6" t="s">
-        <v>583</v>
       </c>
       <c r="H110" s="5" t="s">
         <v>150</v>
       </c>
       <c r="I110" s="6" t="s">
+        <v>583</v>
+      </c>
+      <c r="J110" s="17" t="s">
         <v>584</v>
-      </c>
-      <c r="J110" s="17" t="s">
-        <v>585</v>
       </c>
       <c r="K110" s="4"/>
       <c r="L110" s="4"/>
@@ -7518,32 +7333,32 @@
     </row>
     <row r="111">
       <c r="A111" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>305</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D111" s="11" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E111" s="4"/>
       <c r="F111" s="16" t="s">
+        <v>586</v>
+      </c>
+      <c r="G111" s="6" t="s">
         <v>587</v>
       </c>
-      <c r="G111" s="6" t="s">
+      <c r="H111" s="5" t="s">
         <v>588</v>
       </c>
-      <c r="H111" s="5" t="s">
+      <c r="I111" s="6" t="s">
         <v>589</v>
       </c>
-      <c r="I111" s="6" t="s">
+      <c r="J111" s="17" t="s">
         <v>590</v>
-      </c>
-      <c r="J111" s="17" t="s">
-        <v>591</v>
       </c>
       <c r="K111" s="4"/>
       <c r="L111" s="4"/>
@@ -7564,34 +7379,34 @@
     </row>
     <row r="112">
       <c r="A112" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="B112" s="4" t="s">
         <v>592</v>
-      </c>
-      <c r="B112" s="4" t="s">
-        <v>593</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>505</v>
       </c>
       <c r="D112" s="11" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E112" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F112" s="16" t="s">
+        <v>594</v>
+      </c>
+      <c r="G112" s="6" t="s">
         <v>595</v>
-      </c>
-      <c r="G112" s="6" t="s">
-        <v>596</v>
       </c>
       <c r="H112" s="5" t="s">
         <v>150</v>
       </c>
       <c r="I112" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="J112" s="17" t="s">
         <v>597</v>
-      </c>
-      <c r="J112" s="17" t="s">
-        <v>598</v>
       </c>
       <c r="K112" s="4"/>
       <c r="L112" s="4"/>
@@ -7612,32 +7427,32 @@
     </row>
     <row r="113">
       <c r="A113" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>505</v>
       </c>
       <c r="D113" s="11" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E113" s="4"/>
       <c r="F113" s="16" t="s">
+        <v>600</v>
+      </c>
+      <c r="G113" s="6" t="s">
         <v>601</v>
       </c>
-      <c r="G113" s="6" t="s">
+      <c r="H113" s="5" t="s">
         <v>602</v>
       </c>
-      <c r="H113" s="5" t="s">
+      <c r="I113" s="6" t="s">
         <v>603</v>
       </c>
-      <c r="I113" s="6" t="s">
+      <c r="J113" s="17" t="s">
         <v>604</v>
-      </c>
-      <c r="J113" s="17" t="s">
-        <v>605</v>
       </c>
       <c r="K113" s="4"/>
       <c r="L113" s="4"/>
@@ -7658,7 +7473,7 @@
     </row>
     <row r="114">
       <c r="A114" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>476</v>
@@ -7666,25 +7481,13 @@
       <c r="C114" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="D114" s="11" t="s">
-        <v>606</v>
-      </c>
+      <c r="D114" s="11"/>
       <c r="E114" s="4"/>
-      <c r="F114" s="16" t="s">
-        <v>607</v>
-      </c>
-      <c r="G114" s="6" t="s">
-        <v>608</v>
-      </c>
-      <c r="H114" s="5" t="s">
-        <v>609</v>
-      </c>
-      <c r="I114" s="6" t="s">
-        <v>610</v>
-      </c>
-      <c r="J114" s="17" t="s">
-        <v>611</v>
-      </c>
+      <c r="F114" s="16"/>
+      <c r="G114" s="6"/>
+      <c r="H114" s="5"/>
+      <c r="I114" s="6"/>
+      <c r="J114" s="17"/>
       <c r="K114" s="4"/>
       <c r="L114" s="4"/>
       <c r="M114" s="4"/>
@@ -7704,35 +7507,23 @@
     </row>
     <row r="115">
       <c r="A115" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>439</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>540</v>
-      </c>
-      <c r="D115" s="11" t="s">
-        <v>612</v>
-      </c>
+        <v>539</v>
+      </c>
+      <c r="D115" s="11"/>
       <c r="E115" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F115" s="16" t="s">
-        <v>613</v>
-      </c>
-      <c r="G115" s="6" t="s">
-        <v>614</v>
-      </c>
-      <c r="H115" s="5" t="s">
-        <v>615</v>
-      </c>
-      <c r="I115" s="6" t="s">
-        <v>616</v>
-      </c>
-      <c r="J115" s="17" t="s">
-        <v>617</v>
-      </c>
+      <c r="F115" s="16"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="5"/>
+      <c r="I115" s="6"/>
+      <c r="J115" s="17"/>
       <c r="K115" s="4"/>
       <c r="L115" s="4"/>
       <c r="M115" s="4"/>
@@ -7752,7 +7543,7 @@
     </row>
     <row r="116">
       <c r="A116" s="4" t="s">
-        <v>618</v>
+        <v>605</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>305</v>
@@ -7760,25 +7551,13 @@
       <c r="C116" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="D116" s="11" t="s">
-        <v>619</v>
-      </c>
+      <c r="D116" s="11"/>
       <c r="E116" s="4"/>
-      <c r="F116" s="16" t="s">
-        <v>620</v>
-      </c>
-      <c r="G116" s="6" t="s">
-        <v>621</v>
-      </c>
-      <c r="H116" s="5" t="s">
-        <v>622</v>
-      </c>
-      <c r="I116" s="6" t="s">
-        <v>623</v>
-      </c>
-      <c r="J116" s="17" t="s">
-        <v>624</v>
-      </c>
+      <c r="F116" s="16"/>
+      <c r="G116" s="6"/>
+      <c r="H116" s="5"/>
+      <c r="I116" s="6"/>
+      <c r="J116" s="17"/>
       <c r="K116" s="4"/>
       <c r="L116" s="4"/>
       <c r="M116" s="4"/>
@@ -7798,33 +7577,21 @@
     </row>
     <row r="117">
       <c r="A117" s="4" t="s">
-        <v>618</v>
+        <v>605</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>625</v>
+        <v>606</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="D117" s="11" t="s">
-        <v>626</v>
-      </c>
+      <c r="D117" s="11"/>
       <c r="E117" s="4"/>
-      <c r="F117" s="16" t="s">
-        <v>627</v>
-      </c>
-      <c r="G117" s="6" t="s">
-        <v>628</v>
-      </c>
-      <c r="H117" s="5" t="s">
-        <v>629</v>
-      </c>
-      <c r="I117" s="6" t="s">
-        <v>630</v>
-      </c>
-      <c r="J117" s="17" t="s">
-        <v>631</v>
-      </c>
+      <c r="F117" s="16"/>
+      <c r="G117" s="6"/>
+      <c r="H117" s="5"/>
+      <c r="I117" s="6"/>
+      <c r="J117" s="17"/>
       <c r="K117" s="4"/>
       <c r="L117" s="4"/>
       <c r="M117" s="4"/>
@@ -7844,33 +7611,21 @@
     </row>
     <row r="118">
       <c r="A118" s="4" t="s">
-        <v>618</v>
+        <v>605</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>632</v>
+        <v>607</v>
       </c>
       <c r="C118" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="D118" s="11" t="s">
-        <v>633</v>
-      </c>
+      <c r="D118" s="11"/>
       <c r="E118" s="4"/>
-      <c r="F118" s="16" t="s">
-        <v>634</v>
-      </c>
-      <c r="G118" s="6" t="s">
-        <v>635</v>
-      </c>
-      <c r="H118" s="5" t="s">
-        <v>636</v>
-      </c>
-      <c r="I118" s="6" t="s">
-        <v>637</v>
-      </c>
-      <c r="J118" s="17" t="s">
-        <v>638</v>
-      </c>
+      <c r="F118" s="16"/>
+      <c r="G118" s="6"/>
+      <c r="H118" s="5"/>
+      <c r="I118" s="6"/>
+      <c r="J118" s="17"/>
       <c r="K118" s="4"/>
       <c r="L118" s="4"/>
       <c r="M118" s="4"/>
@@ -7890,35 +7645,23 @@
     </row>
     <row r="119">
       <c r="A119" s="4" t="s">
-        <v>618</v>
+        <v>605</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>639</v>
+        <v>608</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>540</v>
-      </c>
-      <c r="D119" s="11" t="s">
-        <v>640</v>
-      </c>
+        <v>539</v>
+      </c>
+      <c r="D119" s="11"/>
       <c r="E119" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F119" s="16" t="s">
-        <v>641</v>
-      </c>
-      <c r="G119" s="6" t="s">
-        <v>642</v>
-      </c>
-      <c r="H119" s="5" t="s">
-        <v>643</v>
-      </c>
-      <c r="I119" s="6" t="s">
-        <v>644</v>
-      </c>
-      <c r="J119" s="17" t="s">
-        <v>645</v>
-      </c>
+      <c r="F119" s="16"/>
+      <c r="G119" s="6"/>
+      <c r="H119" s="5"/>
+      <c r="I119" s="6"/>
+      <c r="J119" s="17"/>
       <c r="K119" s="4"/>
       <c r="L119" s="4"/>
       <c r="M119" s="4"/>
@@ -7938,33 +7681,21 @@
     </row>
     <row r="120">
       <c r="A120" s="4" t="s">
-        <v>618</v>
+        <v>605</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>646</v>
+        <v>609</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>540</v>
-      </c>
-      <c r="D120" s="11" t="s">
-        <v>647</v>
-      </c>
+        <v>539</v>
+      </c>
+      <c r="D120" s="11"/>
       <c r="E120" s="4"/>
-      <c r="F120" s="16" t="s">
-        <v>648</v>
-      </c>
-      <c r="G120" s="6" t="s">
-        <v>649</v>
-      </c>
-      <c r="H120" s="5" t="s">
-        <v>650</v>
-      </c>
-      <c r="I120" s="6" t="s">
-        <v>651</v>
-      </c>
-      <c r="J120" s="17" t="s">
-        <v>652</v>
-      </c>
+      <c r="F120" s="16"/>
+      <c r="G120" s="6"/>
+      <c r="H120" s="5"/>
+      <c r="I120" s="6"/>
+      <c r="J120" s="17"/>
       <c r="K120" s="4"/>
       <c r="L120" s="4"/>
       <c r="M120" s="4"/>
@@ -7984,33 +7715,21 @@
     </row>
     <row r="121">
       <c r="A121" s="4" t="s">
-        <v>653</v>
+        <v>610</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>654</v>
+        <v>611</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="D121" s="11" t="s">
-        <v>655</v>
-      </c>
+      <c r="D121" s="11"/>
       <c r="E121" s="4"/>
-      <c r="F121" s="16" t="s">
-        <v>656</v>
-      </c>
-      <c r="G121" s="6" t="s">
-        <v>657</v>
-      </c>
-      <c r="H121" s="5" t="s">
-        <v>658</v>
-      </c>
-      <c r="I121" s="6" t="s">
-        <v>659</v>
-      </c>
-      <c r="J121" s="17" t="s">
-        <v>660</v>
-      </c>
+      <c r="F121" s="16"/>
+      <c r="G121" s="6"/>
+      <c r="H121" s="5"/>
+      <c r="I121" s="6"/>
+      <c r="J121" s="17"/>
       <c r="K121" s="4"/>
       <c r="L121" s="4"/>
       <c r="M121" s="4"/>
@@ -8030,33 +7749,21 @@
     </row>
     <row r="122">
       <c r="A122" s="4" t="s">
-        <v>653</v>
+        <v>610</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>661</v>
+        <v>612</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="D122" s="11" t="s">
-        <v>662</v>
-      </c>
+      <c r="D122" s="11"/>
       <c r="E122" s="4"/>
-      <c r="F122" s="16" t="s">
-        <v>663</v>
-      </c>
-      <c r="G122" s="6" t="s">
-        <v>664</v>
-      </c>
-      <c r="H122" s="5" t="s">
-        <v>665</v>
-      </c>
-      <c r="I122" s="6" t="s">
-        <v>666</v>
-      </c>
-      <c r="J122" s="17" t="s">
-        <v>667</v>
-      </c>
+      <c r="F122" s="16"/>
+      <c r="G122" s="6"/>
+      <c r="H122" s="5"/>
+      <c r="I122" s="6"/>
+      <c r="J122" s="17"/>
       <c r="K122" s="4"/>
       <c r="L122" s="4"/>
       <c r="M122" s="4"/>
@@ -8076,35 +7783,23 @@
     </row>
     <row r="123">
       <c r="A123" s="4" t="s">
-        <v>653</v>
+        <v>610</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>668</v>
+        <v>613</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>540</v>
-      </c>
-      <c r="D123" s="11" t="s">
-        <v>669</v>
-      </c>
+        <v>539</v>
+      </c>
+      <c r="D123" s="11"/>
       <c r="E123" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F123" s="16" t="s">
-        <v>670</v>
-      </c>
-      <c r="G123" s="6" t="s">
-        <v>671</v>
-      </c>
-      <c r="H123" s="5" t="s">
-        <v>672</v>
-      </c>
-      <c r="I123" s="6" t="s">
-        <v>673</v>
-      </c>
-      <c r="J123" s="17" t="s">
-        <v>674</v>
-      </c>
+      <c r="F123" s="16"/>
+      <c r="G123" s="6"/>
+      <c r="H123" s="5"/>
+      <c r="I123" s="6"/>
+      <c r="J123" s="17"/>
       <c r="K123" s="4"/>
       <c r="L123" s="4"/>
       <c r="M123" s="4"/>
@@ -8124,13 +7819,13 @@
     </row>
     <row r="124">
       <c r="A124" s="21" t="s">
-        <v>653</v>
+        <v>610</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>668</v>
+        <v>613</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>668</v>
+        <v>613</v>
       </c>
       <c r="D124" s="11"/>
       <c r="E124" s="4"/>
@@ -32550,48 +32245,27 @@
     <hyperlink r:id="rId140" ref="J101"/>
     <hyperlink r:id="rId141" ref="F102"/>
     <hyperlink r:id="rId142" ref="J102"/>
-    <hyperlink r:id="rId143" ref="F103"/>
-    <hyperlink r:id="rId144" ref="J103"/>
-    <hyperlink r:id="rId145" ref="F104"/>
-    <hyperlink r:id="rId146" ref="J104"/>
-    <hyperlink r:id="rId147" ref="F105"/>
-    <hyperlink r:id="rId148" ref="J105"/>
-    <hyperlink r:id="rId149" ref="F106"/>
-    <hyperlink r:id="rId150" ref="J106"/>
-    <hyperlink r:id="rId151" ref="F107"/>
-    <hyperlink r:id="rId152" ref="J107"/>
-    <hyperlink r:id="rId153" ref="F108"/>
-    <hyperlink r:id="rId154" ref="J108"/>
-    <hyperlink r:id="rId155" ref="F109"/>
-    <hyperlink r:id="rId156" ref="J109"/>
-    <hyperlink r:id="rId157" ref="F110"/>
-    <hyperlink r:id="rId158" ref="J110"/>
-    <hyperlink r:id="rId159" ref="F111"/>
-    <hyperlink r:id="rId160" ref="J111"/>
-    <hyperlink r:id="rId161" ref="F112"/>
-    <hyperlink r:id="rId162" ref="J112"/>
-    <hyperlink r:id="rId163" ref="F113"/>
-    <hyperlink r:id="rId164" ref="J113"/>
-    <hyperlink r:id="rId165" ref="F114"/>
-    <hyperlink r:id="rId166" ref="J114"/>
-    <hyperlink r:id="rId167" ref="F115"/>
-    <hyperlink r:id="rId168" ref="J115"/>
-    <hyperlink r:id="rId169" ref="F116"/>
-    <hyperlink r:id="rId170" ref="J116"/>
-    <hyperlink r:id="rId171" ref="F117"/>
-    <hyperlink r:id="rId172" ref="J117"/>
-    <hyperlink r:id="rId173" ref="F118"/>
-    <hyperlink r:id="rId174" ref="J118"/>
-    <hyperlink r:id="rId175" ref="F119"/>
-    <hyperlink r:id="rId176" ref="J119"/>
-    <hyperlink r:id="rId177" ref="F120"/>
-    <hyperlink r:id="rId178" ref="J120"/>
-    <hyperlink r:id="rId179" ref="F121"/>
-    <hyperlink r:id="rId180" ref="J121"/>
-    <hyperlink r:id="rId181" ref="F122"/>
-    <hyperlink r:id="rId182" ref="J122"/>
-    <hyperlink r:id="rId183" ref="F123"/>
-    <hyperlink r:id="rId184" ref="J123"/>
+    <hyperlink r:id="rId143" ref="J103"/>
+    <hyperlink r:id="rId144" ref="F104"/>
+    <hyperlink r:id="rId145" ref="J104"/>
+    <hyperlink r:id="rId146" ref="F105"/>
+    <hyperlink r:id="rId147" ref="J105"/>
+    <hyperlink r:id="rId148" ref="F106"/>
+    <hyperlink r:id="rId149" ref="J106"/>
+    <hyperlink r:id="rId150" ref="F107"/>
+    <hyperlink r:id="rId151" ref="J107"/>
+    <hyperlink r:id="rId152" ref="F108"/>
+    <hyperlink r:id="rId153" ref="J108"/>
+    <hyperlink r:id="rId154" ref="F109"/>
+    <hyperlink r:id="rId155" ref="J109"/>
+    <hyperlink r:id="rId156" ref="F110"/>
+    <hyperlink r:id="rId157" ref="J110"/>
+    <hyperlink r:id="rId158" ref="F111"/>
+    <hyperlink r:id="rId159" ref="J111"/>
+    <hyperlink r:id="rId160" ref="F112"/>
+    <hyperlink r:id="rId161" ref="J112"/>
+    <hyperlink r:id="rId162" ref="F113"/>
+    <hyperlink r:id="rId163" ref="J113"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
finish handler for gorutines
</commit_message>
<xml_diff>
--- a/certificates.xlsx
+++ b/certificates.xlsx
@@ -13,9 +13,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="536">
-  <si>
-    <t>Date</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="537">
+  <si>
+    <t>–</t>
   </si>
   <si>
     <t>Participant</t>
@@ -465,9 +465,6 @@
     <t>0f8a70da32b47c86fa69a39dd522c99b25802700a336d49e16a760eea763f4b1</t>
   </si>
   <si>
-    <t>–</t>
-  </si>
-  <si>
     <t>HCKQDvhlFx194rKcO7OKfVKVHm8iJgs5HBTYDDoPUT1zbt/WBBbpt3FwSlXhjLHeFALjBPeDsJ0+FlqjYJrcedE=</t>
   </si>
   <si>
@@ -1593,6 +1590,9 @@
     <t xml:space="preserve">Anastasia Andreeva</t>
   </si>
   <si>
+    <t>none</t>
+  </si>
+  <si>
     <t xml:space="preserve">Polina Reshetnikova</t>
   </si>
   <si>
@@ -1621,6 +1621,9 @@
   </si>
   <si>
     <t xml:space="preserve">Maksym Cherniak</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -2279,7 +2282,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A1" zoomScale="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
@@ -4104,13 +4107,13 @@
         <v>149</v>
       </c>
       <c r="H47" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I47" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="I47" s="6" t="s">
+      <c r="J47" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="J47" s="9" t="s">
-        <v>152</v>
       </c>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
@@ -4134,31 +4137,31 @@
         <v>143</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>145</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E48" s="15" t="s">
         <v>147</v>
       </c>
       <c r="F48" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="G48" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="G48" s="6" t="s">
+      <c r="H48" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I48" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="H48" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I48" s="6" t="s">
+      <c r="J48" s="9" t="s">
         <v>157</v>
-      </c>
-      <c r="J48" s="9" t="s">
-        <v>158</v>
       </c>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
@@ -4179,34 +4182,34 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>160</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>145</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F49" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="G49" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="G49" s="6" t="s">
+      <c r="H49" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I49" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="H49" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I49" s="6" t="s">
+      <c r="J49" s="17" t="s">
         <v>164</v>
-      </c>
-      <c r="J49" s="17" t="s">
-        <v>165</v>
       </c>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
@@ -4227,32 +4230,32 @@
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>145</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E50" s="7"/>
       <c r="F50" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="G50" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="G50" s="6" t="s">
+      <c r="H50" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H50" s="6" t="s">
+      <c r="I50" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="I50" s="6" t="s">
+      <c r="J50" s="17" t="s">
         <v>171</v>
-      </c>
-      <c r="J50" s="17" t="s">
-        <v>172</v>
       </c>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
@@ -4273,34 +4276,34 @@
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>145</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F51" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G51" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="G51" s="6" t="s">
+      <c r="H51" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I51" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="H51" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I51" s="6" t="s">
+      <c r="J51" s="17" t="s">
         <v>177</v>
-      </c>
-      <c r="J51" s="17" t="s">
-        <v>178</v>
       </c>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
@@ -4321,34 +4324,34 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>145</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F52" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="G52" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="G52" s="6" t="s">
+      <c r="H52" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I52" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="H52" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I52" s="6" t="s">
+      <c r="J52" s="17" t="s">
         <v>183</v>
-      </c>
-      <c r="J52" s="17" t="s">
-        <v>184</v>
       </c>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
@@ -4369,34 +4372,34 @@
     </row>
     <row r="53">
       <c r="A53" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F53" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="G53" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="G53" s="6" t="s">
+      <c r="H53" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I53" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="H53" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I53" s="6" t="s">
+      <c r="J53" s="17" t="s">
         <v>189</v>
-      </c>
-      <c r="J53" s="17" t="s">
-        <v>190</v>
       </c>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
@@ -4417,34 +4420,34 @@
     </row>
     <row r="54">
       <c r="A54" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F54" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="G54" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="G54" s="6" t="s">
+      <c r="H54" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I54" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="H54" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I54" s="6" t="s">
+      <c r="J54" s="17" t="s">
         <v>195</v>
-      </c>
-      <c r="J54" s="17" t="s">
-        <v>196</v>
       </c>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
@@ -4465,34 +4468,34 @@
     </row>
     <row r="55">
       <c r="A55" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F55" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="G55" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="G55" s="6" t="s">
+      <c r="H55" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I55" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="H55" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I55" s="6" t="s">
+      <c r="J55" s="17" t="s">
         <v>201</v>
-      </c>
-      <c r="J55" s="17" t="s">
-        <v>202</v>
       </c>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
@@ -4513,34 +4516,34 @@
     </row>
     <row r="56">
       <c r="A56" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F56" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="G56" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="G56" s="6" t="s">
+      <c r="H56" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I56" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="H56" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I56" s="6" t="s">
+      <c r="J56" s="17" t="s">
         <v>207</v>
-      </c>
-      <c r="J56" s="17" t="s">
-        <v>208</v>
       </c>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
@@ -4561,34 +4564,34 @@
     </row>
     <row r="57">
       <c r="A57" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>160</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F57" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="G57" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="G57" s="6" t="s">
+      <c r="H57" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I57" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="H57" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I57" s="6" t="s">
+      <c r="J57" s="17" t="s">
         <v>164</v>
-      </c>
-      <c r="J57" s="17" t="s">
-        <v>165</v>
       </c>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
@@ -4609,34 +4612,34 @@
     </row>
     <row r="58">
       <c r="A58" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F58" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="G58" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="G58" s="6" t="s">
+      <c r="H58" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I58" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="H58" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I58" s="6" t="s">
+      <c r="J58" s="17" t="s">
         <v>213</v>
-      </c>
-      <c r="J58" s="17" t="s">
-        <v>214</v>
       </c>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
@@ -4657,32 +4660,32 @@
     </row>
     <row r="59">
       <c r="A59" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>216</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E59" s="7"/>
       <c r="F59" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="G59" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="G59" s="6" t="s">
+      <c r="H59" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="H59" s="6" t="s">
+      <c r="I59" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="I59" s="6" t="s">
+      <c r="J59" s="17" t="s">
         <v>221</v>
-      </c>
-      <c r="J59" s="17" t="s">
-        <v>222</v>
       </c>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
@@ -4703,32 +4706,32 @@
     </row>
     <row r="60">
       <c r="A60" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>223</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>224</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E60" s="7"/>
       <c r="F60" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="G60" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="G60" s="6" t="s">
+      <c r="H60" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="H60" s="6" t="s">
+      <c r="I60" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="I60" s="6" t="s">
+      <c r="J60" s="17" t="s">
         <v>229</v>
-      </c>
-      <c r="J60" s="17" t="s">
-        <v>230</v>
       </c>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
@@ -4749,34 +4752,34 @@
     </row>
     <row r="61">
       <c r="A61" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F61" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="G61" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="G61" s="6" t="s">
+      <c r="H61" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I61" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="H61" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I61" s="6" t="s">
+      <c r="J61" s="17" t="s">
         <v>235</v>
-      </c>
-      <c r="J61" s="17" t="s">
-        <v>236</v>
       </c>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
@@ -4797,34 +4800,34 @@
     </row>
     <row r="62">
       <c r="A62" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B62" s="4" t="s">
         <v>237</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>238</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F62" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="G62" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="G62" s="6" t="s">
+      <c r="H62" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="H62" s="6" t="s">
+      <c r="I62" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="I62" s="6" t="s">
+      <c r="J62" s="17" t="s">
         <v>243</v>
-      </c>
-      <c r="J62" s="17" t="s">
-        <v>244</v>
       </c>
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
@@ -4845,34 +4848,34 @@
     </row>
     <row r="63">
       <c r="A63" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>245</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>246</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F63" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="G63" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="G63" s="6" t="s">
+      <c r="H63" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="H63" s="6" t="s">
+      <c r="I63" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="I63" s="6" t="s">
+      <c r="J63" s="17" t="s">
         <v>251</v>
-      </c>
-      <c r="J63" s="17" t="s">
-        <v>252</v>
       </c>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
@@ -4893,32 +4896,32 @@
     </row>
     <row r="64">
       <c r="A64" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>253</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>254</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E64" s="7"/>
       <c r="F64" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="G64" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="G64" s="6" t="s">
+      <c r="H64" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="H64" s="6" t="s">
+      <c r="I64" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="I64" s="6" t="s">
+      <c r="J64" s="17" t="s">
         <v>259</v>
-      </c>
-      <c r="J64" s="17" t="s">
-        <v>260</v>
       </c>
       <c r="K64" s="4"/>
       <c r="L64" s="4"/>
@@ -4939,32 +4942,32 @@
     </row>
     <row r="65">
       <c r="A65" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E65" s="7"/>
       <c r="F65" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="G65" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="G65" s="6" t="s">
+      <c r="H65" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="H65" s="6" t="s">
+      <c r="I65" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="I65" s="6" t="s">
+      <c r="J65" s="17" t="s">
         <v>266</v>
-      </c>
-      <c r="J65" s="17" t="s">
-        <v>267</v>
       </c>
       <c r="K65" s="4"/>
       <c r="L65" s="4"/>
@@ -4985,32 +4988,32 @@
     </row>
     <row r="66">
       <c r="A66" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>268</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>269</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E66" s="7"/>
       <c r="F66" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="G66" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="G66" s="6" t="s">
+      <c r="H66" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="H66" s="6" t="s">
+      <c r="I66" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="I66" s="6" t="s">
+      <c r="J66" s="17" t="s">
         <v>274</v>
-      </c>
-      <c r="J66" s="17" t="s">
-        <v>275</v>
       </c>
       <c r="K66" s="4"/>
       <c r="L66" s="4"/>
@@ -5031,32 +5034,32 @@
     </row>
     <row r="67">
       <c r="A67" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E67" s="7"/>
       <c r="F67" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="G67" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="G67" s="6" t="s">
+      <c r="H67" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="H67" s="6" t="s">
+      <c r="I67" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="I67" s="6" t="s">
+      <c r="J67" s="17" t="s">
         <v>281</v>
-      </c>
-      <c r="J67" s="17" t="s">
-        <v>282</v>
       </c>
       <c r="K67" s="4"/>
       <c r="L67" s="4"/>
@@ -5077,34 +5080,34 @@
     </row>
     <row r="68">
       <c r="A68" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B68" s="4" t="s">
         <v>283</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>284</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F68" s="16" t="s">
+        <v>285</v>
+      </c>
+      <c r="G68" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="G68" s="6" t="s">
+      <c r="H68" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I68" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="H68" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I68" s="6" t="s">
+      <c r="J68" s="17" t="s">
         <v>288</v>
-      </c>
-      <c r="J68" s="17" t="s">
-        <v>289</v>
       </c>
       <c r="K68" s="4"/>
       <c r="L68" s="4"/>
@@ -5125,32 +5128,32 @@
     </row>
     <row r="69">
       <c r="A69" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>290</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>291</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E69" s="4"/>
       <c r="F69" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="G69" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="G69" s="6" t="s">
+      <c r="H69" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="H69" s="6" t="s">
+      <c r="I69" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="I69" s="6" t="s">
+      <c r="J69" s="17" t="s">
         <v>296</v>
-      </c>
-      <c r="J69" s="17" t="s">
-        <v>297</v>
       </c>
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
@@ -5171,32 +5174,32 @@
     </row>
     <row r="70">
       <c r="A70" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E70" s="4"/>
       <c r="F70" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="G70" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="G70" s="6" t="s">
+      <c r="H70" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="H70" s="6" t="s">
+      <c r="I70" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="I70" s="6" t="s">
+      <c r="J70" s="17" t="s">
         <v>303</v>
-      </c>
-      <c r="J70" s="17" t="s">
-        <v>304</v>
       </c>
       <c r="K70" s="4"/>
       <c r="L70" s="4"/>
@@ -5217,32 +5220,32 @@
     </row>
     <row r="71">
       <c r="A71" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="G71" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="G71" s="6" t="s">
+      <c r="H71" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="H71" s="6" t="s">
+      <c r="I71" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="I71" s="6" t="s">
+      <c r="J71" s="17" t="s">
         <v>310</v>
-      </c>
-      <c r="J71" s="17" t="s">
-        <v>311</v>
       </c>
       <c r="K71" s="4"/>
       <c r="L71" s="4"/>
@@ -5263,34 +5266,34 @@
     </row>
     <row r="72">
       <c r="A72" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F72" s="16" t="s">
+        <v>313</v>
+      </c>
+      <c r="G72" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="G72" s="6" t="s">
+      <c r="H72" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I72" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="H72" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I72" s="6" t="s">
+      <c r="J72" s="17" t="s">
         <v>316</v>
-      </c>
-      <c r="J72" s="17" t="s">
-        <v>317</v>
       </c>
       <c r="K72" s="4"/>
       <c r="L72" s="4"/>
@@ -5311,32 +5314,32 @@
     </row>
     <row r="73">
       <c r="A73" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="B73" s="4" t="s">
         <v>318</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>319</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="G73" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="G73" s="6" t="s">
+      <c r="H73" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="H73" s="6" t="s">
+      <c r="I73" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="I73" s="6" t="s">
+      <c r="J73" s="17" t="s">
         <v>324</v>
-      </c>
-      <c r="J73" s="17" t="s">
-        <v>325</v>
       </c>
       <c r="K73" s="4"/>
       <c r="L73" s="4"/>
@@ -5357,34 +5360,34 @@
     </row>
     <row r="74">
       <c r="A74" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F74" s="16" t="s">
+        <v>327</v>
+      </c>
+      <c r="G74" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="G74" s="6" t="s">
+      <c r="H74" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="H74" s="6" t="s">
+      <c r="I74" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="I74" s="6" t="s">
+      <c r="J74" s="17" t="s">
         <v>331</v>
-      </c>
-      <c r="J74" s="17" t="s">
-        <v>332</v>
       </c>
       <c r="K74" s="4"/>
       <c r="L74" s="4"/>
@@ -5405,34 +5408,34 @@
     </row>
     <row r="75">
       <c r="A75" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B75" s="4" t="s">
         <v>333</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>334</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F75" s="16" t="s">
+        <v>335</v>
+      </c>
+      <c r="G75" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="G75" s="6" t="s">
+      <c r="H75" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="H75" s="6" t="s">
+      <c r="I75" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="I75" s="6" t="s">
+      <c r="J75" s="17" t="s">
         <v>339</v>
-      </c>
-      <c r="J75" s="17" t="s">
-        <v>340</v>
       </c>
       <c r="K75" s="4"/>
       <c r="L75" s="4"/>
@@ -5453,34 +5456,34 @@
     </row>
     <row r="76">
       <c r="A76" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F76" s="16" t="s">
+        <v>342</v>
+      </c>
+      <c r="G76" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="G76" s="6" t="s">
+      <c r="H76" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I76" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="H76" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I76" s="6" t="s">
+      <c r="J76" s="17" t="s">
         <v>345</v>
-      </c>
-      <c r="J76" s="17" t="s">
-        <v>346</v>
       </c>
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
@@ -5501,34 +5504,34 @@
     </row>
     <row r="77">
       <c r="A77" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F77" s="16" t="s">
+        <v>348</v>
+      </c>
+      <c r="G77" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="G77" s="6" t="s">
+      <c r="H77" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I77" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="H77" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I77" s="6" t="s">
+      <c r="J77" s="17" t="s">
         <v>351</v>
-      </c>
-      <c r="J77" s="17" t="s">
-        <v>352</v>
       </c>
       <c r="K77" s="4"/>
       <c r="L77" s="4"/>
@@ -5549,34 +5552,34 @@
     </row>
     <row r="78">
       <c r="A78" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="B78" s="4" t="s">
         <v>353</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>354</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F78" s="16" t="s">
+        <v>355</v>
+      </c>
+      <c r="G78" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="G78" s="6" t="s">
+      <c r="H78" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I78" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="H78" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I78" s="6" t="s">
+      <c r="J78" s="17" t="s">
         <v>358</v>
-      </c>
-      <c r="J78" s="17" t="s">
-        <v>359</v>
       </c>
       <c r="K78" s="4"/>
       <c r="L78" s="4"/>
@@ -5597,32 +5600,32 @@
     </row>
     <row r="79">
       <c r="A79" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="G79" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="G79" s="6" t="s">
+      <c r="H79" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="H79" s="6" t="s">
+      <c r="I79" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="I79" s="6" t="s">
+      <c r="J79" s="17" t="s">
         <v>365</v>
-      </c>
-      <c r="J79" s="17" t="s">
-        <v>366</v>
       </c>
       <c r="K79" s="4"/>
       <c r="L79" s="4"/>
@@ -5643,32 +5646,32 @@
     </row>
     <row r="80">
       <c r="A80" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="16" t="s">
+        <v>368</v>
+      </c>
+      <c r="G80" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="G80" s="6" t="s">
+      <c r="H80" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="H80" s="6" t="s">
+      <c r="I80" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="I80" s="6" t="s">
+      <c r="J80" s="17" t="s">
         <v>372</v>
-      </c>
-      <c r="J80" s="17" t="s">
-        <v>373</v>
       </c>
       <c r="K80" s="4"/>
       <c r="L80" s="4"/>
@@ -5689,32 +5692,32 @@
     </row>
     <row r="81">
       <c r="A81" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E81" s="4"/>
       <c r="F81" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="G81" s="6" t="s">
         <v>376</v>
       </c>
-      <c r="G81" s="6" t="s">
+      <c r="H81" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="H81" s="6" t="s">
+      <c r="I81" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="I81" s="6" t="s">
+      <c r="J81" s="17" t="s">
         <v>379</v>
-      </c>
-      <c r="J81" s="17" t="s">
-        <v>380</v>
       </c>
       <c r="K81" s="4"/>
       <c r="L81" s="4"/>
@@ -5735,34 +5738,34 @@
     </row>
     <row r="82">
       <c r="A82" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="B82" s="4" t="s">
         <v>381</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>382</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E82" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F82" s="16" t="s">
+        <v>383</v>
+      </c>
+      <c r="G82" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="G82" s="6" t="s">
+      <c r="H82" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="H82" s="6" t="s">
+      <c r="I82" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="I82" s="6" t="s">
+      <c r="J82" s="17" t="s">
         <v>387</v>
-      </c>
-      <c r="J82" s="17" t="s">
-        <v>388</v>
       </c>
       <c r="K82" s="4"/>
       <c r="L82" s="4"/>
@@ -5783,34 +5786,34 @@
     </row>
     <row r="83">
       <c r="A83" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F83" s="16" t="s">
+        <v>390</v>
+      </c>
+      <c r="G83" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="G83" s="6" t="s">
+      <c r="H83" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="H83" s="6" t="s">
+      <c r="I83" s="6" t="s">
         <v>393</v>
       </c>
-      <c r="I83" s="6" t="s">
+      <c r="J83" s="17" t="s">
         <v>394</v>
-      </c>
-      <c r="J83" s="17" t="s">
-        <v>395</v>
       </c>
       <c r="K83" s="4"/>
       <c r="L83" s="4"/>
@@ -5831,32 +5834,32 @@
     </row>
     <row r="84">
       <c r="A84" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="16" t="s">
+        <v>397</v>
+      </c>
+      <c r="G84" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="G84" s="6" t="s">
+      <c r="H84" s="6" t="s">
         <v>399</v>
       </c>
-      <c r="H84" s="6" t="s">
+      <c r="I84" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="I84" s="6" t="s">
+      <c r="J84" s="17" t="s">
         <v>401</v>
-      </c>
-      <c r="J84" s="17" t="s">
-        <v>402</v>
       </c>
       <c r="K84" s="4"/>
       <c r="L84" s="4"/>
@@ -5877,34 +5880,34 @@
     </row>
     <row r="85">
       <c r="A85" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="B85" s="4" t="s">
         <v>403</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>404</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F85" s="16" t="s">
+        <v>405</v>
+      </c>
+      <c r="G85" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="G85" s="6" t="s">
+      <c r="H85" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I85" s="6" t="s">
         <v>407</v>
       </c>
-      <c r="H85" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I85" s="6" t="s">
+      <c r="J85" s="17" t="s">
         <v>408</v>
-      </c>
-      <c r="J85" s="17" t="s">
-        <v>409</v>
       </c>
       <c r="K85" s="4"/>
       <c r="L85" s="4"/>
@@ -5925,32 +5928,32 @@
     </row>
     <row r="86">
       <c r="A86" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="16" t="s">
+        <v>411</v>
+      </c>
+      <c r="G86" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="G86" s="6" t="s">
+      <c r="H86" s="6" t="s">
         <v>413</v>
       </c>
-      <c r="H86" s="6" t="s">
+      <c r="I86" s="6" t="s">
         <v>414</v>
       </c>
-      <c r="I86" s="6" t="s">
+      <c r="J86" s="17" t="s">
         <v>415</v>
-      </c>
-      <c r="J86" s="17" t="s">
-        <v>416</v>
       </c>
       <c r="K86" s="4"/>
       <c r="L86" s="4"/>
@@ -5971,32 +5974,32 @@
     </row>
     <row r="87">
       <c r="A87" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="16" t="s">
+        <v>418</v>
+      </c>
+      <c r="G87" s="6" t="s">
         <v>419</v>
       </c>
-      <c r="G87" s="6" t="s">
+      <c r="H87" s="6" t="s">
         <v>420</v>
       </c>
-      <c r="H87" s="6" t="s">
+      <c r="I87" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="J87" s="17" t="s">
         <v>421</v>
-      </c>
-      <c r="I87" s="6" t="s">
-        <v>415</v>
-      </c>
-      <c r="J87" s="17" t="s">
-        <v>422</v>
       </c>
       <c r="K87" s="4"/>
       <c r="L87" s="4"/>
@@ -6017,32 +6020,32 @@
     </row>
     <row r="88">
       <c r="A88" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="B88" s="4" t="s">
         <v>423</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>424</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="16" t="s">
+        <v>425</v>
+      </c>
+      <c r="G88" s="6" t="s">
         <v>426</v>
       </c>
-      <c r="G88" s="6" t="s">
+      <c r="H88" s="6" t="s">
         <v>427</v>
       </c>
-      <c r="H88" s="6" t="s">
+      <c r="I88" s="6" t="s">
         <v>428</v>
       </c>
-      <c r="I88" s="6" t="s">
+      <c r="J88" s="17" t="s">
         <v>429</v>
-      </c>
-      <c r="J88" s="17" t="s">
-        <v>430</v>
       </c>
       <c r="K88" s="4"/>
       <c r="L88" s="4"/>
@@ -6063,34 +6066,34 @@
     </row>
     <row r="89">
       <c r="A89" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E89" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F89" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="G89" s="6" t="s">
         <v>433</v>
       </c>
-      <c r="G89" s="6" t="s">
+      <c r="H89" s="6" t="s">
         <v>434</v>
       </c>
-      <c r="H89" s="6" t="s">
+      <c r="I89" s="6" t="s">
         <v>435</v>
       </c>
-      <c r="I89" s="6" t="s">
+      <c r="J89" s="17" t="s">
         <v>436</v>
-      </c>
-      <c r="J89" s="17" t="s">
-        <v>437</v>
       </c>
       <c r="K89" s="4"/>
       <c r="L89" s="4"/>
@@ -6111,34 +6114,34 @@
     </row>
     <row r="90">
       <c r="A90" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="B90" s="4" t="s">
         <v>438</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>439</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E90" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F90" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="G90" s="6" t="s">
         <v>441</v>
       </c>
-      <c r="G90" s="6" t="s">
+      <c r="H90" s="6" t="s">
         <v>442</v>
       </c>
-      <c r="H90" s="6" t="s">
+      <c r="I90" s="6" t="s">
         <v>443</v>
       </c>
-      <c r="I90" s="6" t="s">
+      <c r="J90" s="17" t="s">
         <v>444</v>
-      </c>
-      <c r="J90" s="17" t="s">
-        <v>445</v>
       </c>
       <c r="K90" s="4"/>
       <c r="L90" s="4"/>
@@ -6159,32 +6162,32 @@
     </row>
     <row r="91">
       <c r="A91" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="B91" s="4" t="s">
         <v>446</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>447</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E91" s="4"/>
       <c r="F91" s="16" t="s">
+        <v>448</v>
+      </c>
+      <c r="G91" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="G91" s="6" t="s">
+      <c r="H91" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="H91" s="6" t="s">
+      <c r="I91" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="I91" s="6" t="s">
+      <c r="J91" s="17" t="s">
         <v>452</v>
-      </c>
-      <c r="J91" s="17" t="s">
-        <v>453</v>
       </c>
       <c r="K91" s="4"/>
       <c r="L91" s="4"/>
@@ -6205,32 +6208,32 @@
     </row>
     <row r="92">
       <c r="A92" s="4" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="16" t="s">
+        <v>455</v>
+      </c>
+      <c r="G92" s="6" t="s">
         <v>456</v>
       </c>
-      <c r="G92" s="6" t="s">
+      <c r="H92" s="6" t="s">
         <v>457</v>
       </c>
-      <c r="H92" s="6" t="s">
+      <c r="I92" s="6" t="s">
         <v>458</v>
       </c>
-      <c r="I92" s="6" t="s">
+      <c r="J92" s="17" t="s">
         <v>459</v>
-      </c>
-      <c r="J92" s="17" t="s">
-        <v>460</v>
       </c>
       <c r="K92" s="4"/>
       <c r="L92" s="4"/>
@@ -6251,34 +6254,34 @@
     </row>
     <row r="93">
       <c r="A93" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="B93" s="4" t="s">
         <v>461</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>462</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E93" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F93" s="16" t="s">
+        <v>463</v>
+      </c>
+      <c r="G93" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="G93" s="6" t="s">
+      <c r="H93" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I93" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="H93" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I93" s="6" t="s">
+      <c r="J93" s="17" t="s">
         <v>466</v>
-      </c>
-      <c r="J93" s="17" t="s">
-        <v>467</v>
       </c>
       <c r="K93" s="4"/>
       <c r="L93" s="4"/>
@@ -6299,32 +6302,32 @@
     </row>
     <row r="94">
       <c r="A94" s="4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E94" s="4"/>
       <c r="F94" s="16" t="s">
+        <v>469</v>
+      </c>
+      <c r="G94" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="G94" s="6" t="s">
+      <c r="H94" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="H94" s="6" t="s">
+      <c r="I94" s="6" t="s">
         <v>472</v>
       </c>
-      <c r="I94" s="6" t="s">
+      <c r="J94" s="17" t="s">
         <v>473</v>
-      </c>
-      <c r="J94" s="17" t="s">
-        <v>474</v>
       </c>
       <c r="K94" s="4"/>
       <c r="L94" s="4"/>
@@ -6345,34 +6348,34 @@
     </row>
     <row r="95">
       <c r="A95" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="B95" s="4" t="s">
         <v>475</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>476</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F95" s="16" t="s">
+        <v>477</v>
+      </c>
+      <c r="G95" s="6" t="s">
         <v>478</v>
       </c>
-      <c r="G95" s="6" t="s">
+      <c r="H95" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I95" s="6" t="s">
         <v>479</v>
       </c>
-      <c r="H95" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I95" s="6" t="s">
+      <c r="J95" s="17" t="s">
         <v>480</v>
-      </c>
-      <c r="J95" s="17" t="s">
-        <v>481</v>
       </c>
       <c r="K95" s="4"/>
       <c r="L95" s="4"/>
@@ -6393,32 +6396,32 @@
     </row>
     <row r="96">
       <c r="A96" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E96" s="4"/>
       <c r="F96" s="16" t="s">
+        <v>483</v>
+      </c>
+      <c r="G96" s="6" t="s">
         <v>484</v>
       </c>
-      <c r="G96" s="6" t="s">
+      <c r="H96" s="6" t="s">
         <v>485</v>
       </c>
-      <c r="H96" s="6" t="s">
+      <c r="I96" s="6" t="s">
         <v>486</v>
       </c>
-      <c r="I96" s="6" t="s">
+      <c r="J96" s="17" t="s">
         <v>487</v>
-      </c>
-      <c r="J96" s="17" t="s">
-        <v>488</v>
       </c>
       <c r="K96" s="4"/>
       <c r="L96" s="4"/>
@@ -6439,34 +6442,34 @@
     </row>
     <row r="97">
       <c r="A97" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E97" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F97" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="G97" s="6" t="s">
         <v>491</v>
       </c>
-      <c r="G97" s="6" t="s">
+      <c r="H97" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I97" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="H97" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I97" s="6" t="s">
+      <c r="J97" s="17" t="s">
         <v>493</v>
-      </c>
-      <c r="J97" s="17" t="s">
-        <v>494</v>
       </c>
       <c r="K97" s="4"/>
       <c r="L97" s="4"/>
@@ -6487,34 +6490,34 @@
     </row>
     <row r="98">
       <c r="A98" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="B98" s="4" t="s">
         <v>495</v>
-      </c>
-      <c r="B98" s="4" t="s">
-        <v>496</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D98" s="18" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E98" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F98" s="19" t="s">
+        <v>497</v>
+      </c>
+      <c r="G98" s="20" t="s">
         <v>498</v>
       </c>
-      <c r="G98" s="20" t="s">
+      <c r="H98" s="20" t="s">
         <v>499</v>
       </c>
-      <c r="H98" s="20" t="s">
+      <c r="I98" s="20" t="s">
         <v>500</v>
       </c>
-      <c r="I98" s="20" t="s">
+      <c r="J98" s="19" t="s">
         <v>501</v>
-      </c>
-      <c r="J98" s="19" t="s">
-        <v>502</v>
       </c>
       <c r="K98" s="4"/>
       <c r="L98" s="4"/>
@@ -6535,34 +6538,34 @@
     </row>
     <row r="99">
       <c r="A99" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="B99" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="C99" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="C99" s="4" t="s">
+      <c r="D99" s="11" t="s">
         <v>505</v>
-      </c>
-      <c r="D99" s="11" t="s">
-        <v>506</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F99" s="16" t="s">
+        <v>506</v>
+      </c>
+      <c r="G99" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="G99" s="6" t="s">
+      <c r="H99" s="5" t="s">
         <v>508</v>
       </c>
-      <c r="H99" s="5" t="s">
+      <c r="I99" s="6" t="s">
         <v>509</v>
       </c>
-      <c r="I99" s="6" t="s">
+      <c r="J99" s="17" t="s">
         <v>510</v>
-      </c>
-      <c r="J99" s="17" t="s">
-        <v>511</v>
       </c>
       <c r="K99" s="4"/>
       <c r="L99" s="4"/>
@@ -6583,13 +6586,13 @@
     </row>
     <row r="100">
       <c r="A100" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B100" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="B100" s="4" t="s">
-        <v>513</v>
-      </c>
       <c r="C100" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D100" s="11"/>
       <c r="E100" s="5"/>
@@ -6617,13 +6620,13 @@
     </row>
     <row r="101">
       <c r="A101" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D101" s="11"/>
       <c r="E101" s="4"/>
@@ -6651,13 +6654,13 @@
     </row>
     <row r="102">
       <c r="A102" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D102" s="11"/>
       <c r="E102" s="4"/>
@@ -6685,13 +6688,13 @@
     </row>
     <row r="103">
       <c r="A103" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D103" s="11"/>
       <c r="E103" s="4"/>
@@ -6719,13 +6722,13 @@
     </row>
     <row r="104">
       <c r="A104" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D104" s="11"/>
       <c r="E104" s="4"/>
@@ -6753,13 +6756,13 @@
     </row>
     <row r="105">
       <c r="A105" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D105" s="11"/>
       <c r="E105" s="5"/>
@@ -6787,13 +6790,13 @@
     </row>
     <row r="106">
       <c r="A106" s="4" t="s">
+        <v>517</v>
+      </c>
+      <c r="B106" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="B106" s="4" t="s">
-        <v>519</v>
-      </c>
       <c r="C106" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D106" s="11"/>
       <c r="E106" s="4"/>
@@ -6821,13 +6824,13 @@
     </row>
     <row r="107">
       <c r="A107" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D107" s="11"/>
       <c r="E107" s="4"/>
@@ -6855,13 +6858,13 @@
     </row>
     <row r="108">
       <c r="A108" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="B108" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="B108" s="4" t="s">
-        <v>521</v>
-      </c>
       <c r="C108" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D108" s="11"/>
       <c r="E108" s="4"/>
@@ -6889,13 +6892,13 @@
     </row>
     <row r="109">
       <c r="A109" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D109" s="11"/>
       <c r="E109" s="4"/>
@@ -6923,13 +6926,13 @@
     </row>
     <row r="110">
       <c r="A110" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D110" s="11"/>
       <c r="E110" s="4"/>
@@ -6957,13 +6960,13 @@
     </row>
     <row r="111">
       <c r="A111" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D111" s="11"/>
       <c r="E111" s="4"/>
@@ -6991,19 +6994,21 @@
     </row>
     <row r="112">
       <c r="A112" s="4" t="s">
+        <v>523</v>
+      </c>
+      <c r="B112" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="B112" s="4" t="s">
-        <v>525</v>
-      </c>
       <c r="C112" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D112" s="11"/>
       <c r="E112" s="4"/>
       <c r="F112" s="16"/>
       <c r="G112" s="6"/>
-      <c r="H112" s="5"/>
+      <c r="H112" s="5" t="s">
+        <v>525</v>
+      </c>
       <c r="I112" s="6"/>
       <c r="J112" s="17"/>
       <c r="K112" s="4"/>
@@ -7025,13 +7030,13 @@
     </row>
     <row r="113">
       <c r="A113" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>526</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D113" s="11"/>
       <c r="E113" s="4"/>
@@ -7059,13 +7064,13 @@
     </row>
     <row r="114">
       <c r="A114" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D114" s="11"/>
       <c r="E114" s="4"/>
@@ -7093,13 +7098,13 @@
     </row>
     <row r="115">
       <c r="A115" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D115" s="11"/>
       <c r="E115" s="5" t="s">
@@ -7132,16 +7137,18 @@
         <v>527</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D116" s="11"/>
       <c r="E116" s="4"/>
       <c r="F116" s="16"/>
       <c r="G116" s="6"/>
-      <c r="H116" s="5"/>
+      <c r="H116" s="5" t="s">
+        <v>525</v>
+      </c>
       <c r="I116" s="6"/>
       <c r="J116" s="17"/>
       <c r="K116" s="4"/>
@@ -7169,7 +7176,7 @@
         <v>528</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D117" s="11"/>
       <c r="E117" s="4"/>
@@ -7203,7 +7210,7 @@
         <v>529</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D118" s="11"/>
       <c r="E118" s="4"/>
@@ -7237,7 +7244,7 @@
         <v>530</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D119" s="11"/>
       <c r="E119" s="5" t="s">
@@ -7273,7 +7280,7 @@
         <v>531</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D120" s="11"/>
       <c r="E120" s="4"/>
@@ -7307,13 +7314,15 @@
         <v>533</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D121" s="11"/>
       <c r="E121" s="4"/>
       <c r="F121" s="16"/>
       <c r="G121" s="6"/>
-      <c r="H121" s="5"/>
+      <c r="H121" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="I121" s="6"/>
       <c r="J121" s="17"/>
       <c r="K121" s="4"/>
@@ -7341,13 +7350,15 @@
         <v>534</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D122" s="11"/>
       <c r="E122" s="4"/>
       <c r="F122" s="16"/>
       <c r="G122" s="6"/>
-      <c r="H122" s="5"/>
+      <c r="H122" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="I122" s="6"/>
       <c r="J122" s="17"/>
       <c r="K122" s="4"/>
@@ -7375,7 +7386,7 @@
         <v>535</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D123" s="11"/>
       <c r="E123" s="5" t="s">
@@ -7383,7 +7394,9 @@
       </c>
       <c r="F123" s="16"/>
       <c r="G123" s="6"/>
-      <c r="H123" s="5"/>
+      <c r="H123" s="5" t="s">
+        <v>536</v>
+      </c>
       <c r="I123" s="6"/>
       <c r="J123" s="17"/>
       <c r="K123" s="4"/>

</xml_diff>

<commit_message>
fix error with losing data
</commit_message>
<xml_diff>
--- a/certificates.xlsx
+++ b/certificates.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="536">
   <si>
     <t>–</t>
   </si>
@@ -1588,9 +1588,6 @@
   </si>
   <si>
     <t xml:space="preserve">Anastasia Andreeva</t>
-  </si>
-  <si>
-    <t>none</t>
   </si>
   <si>
     <t xml:space="preserve">Polina Reshetnikova</t>
@@ -7006,9 +7003,7 @@
       <c r="E112" s="4"/>
       <c r="F112" s="16"/>
       <c r="G112" s="6"/>
-      <c r="H112" s="5" t="s">
-        <v>525</v>
-      </c>
+      <c r="H112" s="5"/>
       <c r="I112" s="6"/>
       <c r="J112" s="17"/>
       <c r="K112" s="4"/>
@@ -7033,7 +7028,7 @@
         <v>523</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>504</v>
@@ -7134,7 +7129,7 @@
     </row>
     <row r="116">
       <c r="A116" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>304</v>
@@ -7146,9 +7141,7 @@
       <c r="E116" s="4"/>
       <c r="F116" s="16"/>
       <c r="G116" s="6"/>
-      <c r="H116" s="5" t="s">
-        <v>525</v>
-      </c>
+      <c r="H116" s="5"/>
       <c r="I116" s="6"/>
       <c r="J116" s="17"/>
       <c r="K116" s="4"/>
@@ -7170,10 +7163,10 @@
     </row>
     <row r="117">
       <c r="A117" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="B117" s="4" t="s">
         <v>527</v>
-      </c>
-      <c r="B117" s="4" t="s">
-        <v>528</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>504</v>
@@ -7204,10 +7197,10 @@
     </row>
     <row r="118">
       <c r="A118" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C118" s="4" t="s">
         <v>504</v>
@@ -7238,10 +7231,10 @@
     </row>
     <row r="119">
       <c r="A119" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>516</v>
@@ -7274,10 +7267,10 @@
     </row>
     <row r="120">
       <c r="A120" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>516</v>
@@ -7308,10 +7301,10 @@
     </row>
     <row r="121">
       <c r="A121" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="B121" s="4" t="s">
         <v>532</v>
-      </c>
-      <c r="B121" s="4" t="s">
-        <v>533</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>504</v>
@@ -7344,10 +7337,10 @@
     </row>
     <row r="122">
       <c r="A122" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>504</v>
@@ -7380,10 +7373,10 @@
     </row>
     <row r="123">
       <c r="A123" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C123" s="4" t="s">
         <v>516</v>
@@ -7395,7 +7388,7 @@
       <c r="F123" s="16"/>
       <c r="G123" s="6"/>
       <c r="H123" s="5" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I123" s="6"/>
       <c r="J123" s="17"/>
@@ -7418,13 +7411,13 @@
     </row>
     <row r="124">
       <c r="A124" s="21" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D124" s="11"/>
       <c r="E124" s="4"/>

</xml_diff>